<commit_message>
update oct 9 2020
</commit_message>
<xml_diff>
--- a/filmstarts/Filmstarts_20201005.xlsx
+++ b/filmstarts/Filmstarts_20201005.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:J51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -573,7 +573,7 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>www.youtube.com/watch?v=3Qqy6IeVum8</t>
+          <t>www.youtube.com/watch?v=bpc7ScQkIvs</t>
         </is>
       </c>
     </row>
@@ -861,7 +861,7 @@
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>www.youtube.com/watch?v=2BqgGqQDuxo</t>
+          <t>www.youtube.com/watch?v=JwG3kZSox2g</t>
         </is>
       </c>
     </row>
@@ -1303,7 +1303,7 @@
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>www.youtube.com/watch?v=3Sq7qhsaB2A</t>
+          <t>www.youtube.com/watch?v=y1wBNlYm_YM</t>
         </is>
       </c>
     </row>
@@ -1445,7 +1445,7 @@
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>www.youtube.com/watch?v=70KNXfa052g</t>
+          <t>www.youtube.com/watch?v=cgoTUHHGHJk</t>
         </is>
       </c>
     </row>
@@ -1592,6 +1592,1324 @@
       <c r="J24" t="inlineStr">
         <is>
           <t>www.youtube.com/watch?v=23pNPezU1RI</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>15.10.2020</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Astronaut </t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Shelagh McLeod</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Richard Dreyfuss, Lyriq Bent, Krista Bridges, Colm Feore, Richie Lawrence</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>https://www.kino-zeit.de/node/50228</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>https://www.kino-zeit.de/sites/default/files/styles/2560_x_1440_header_/public/2020-07/astronaut_3.jpg</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>JETS Filmverleih &amp; Vertrieb</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>Kanada</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>www.youtube.com/watch?v=FLnE15vAHcA</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>15.10.2020</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Bruno - Die lange Heimreise </t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Karl Golden</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Diarmaid Murtagh, Woody Norman, Seun Shote, Scarlett Alice Johnson</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>https://www.kino-zeit.de/node/48854</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>https://www.kino-zeit.de/sites/default/files/styles/2560_x_1440_header_/public/2020-08/bruno_7_daniel_andizzy_searching_copyrightfilmperlen.jpg</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>Filmperlen</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>Großbritannien</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>www.youtube.com/watch?v=_rpLj7zYEYI</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>18.10.2020</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Chernobyl: Abyss </t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Danila Kozlovsky</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Oksana Akinshina, Danila Kozlowskj, Filipp Avdeew</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>https://www.kino-zeit.de/node/50781</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>https://www.kino-zeit.de/sites/default/files/styles/2560_x_1440_header_/public/2020-09/chernobyl_abyss_2.jpg</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>Capelight Pictures / Central</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>Russland</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>www.youtube.com/watch?v=amiO_cqRKis</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>15.10.2020</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Der Bär in mir </t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Roman Droux</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr"/>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>https://www.kino-zeit.de/node/50292</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>https://www.kino-zeit.de/sites/default/files/styles/2560_x_1440_header_/public/2020-07/der_bar_in_mir_2.jpg</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>MFA + Filmdistribution</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>Schweiz</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>www.youtube.com/watch?v=JYAGKtI94eI</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>15.10.2020</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Der geheime Garten </t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Marc Munden</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Colin Firth, Maeve Dermody, Julie Walters, Dixie Egerickx</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>https://www.kino-zeit.de/node/47584</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>https://www.kino-zeit.de/sites/default/files/styles/2560_x_1440_header_/public/2020-02/dergeheimegarten_003.jpg</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>STUDIOCANAL GmbH Filmverleih</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>Großbritannien, Frankreich</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>www.youtube.com/watch?v=ucZlnduCbL0</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>16.10.2020</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I Am Greta </t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Nathan Grossman</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Greta Thunberg</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>https://www.kino-zeit.de/node/50550</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>https://www.kino-zeit.de/sites/default/files/styles/2560_x_1440_header_/public/2020-08/Greta_Biennale.jpg</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>Filmwelt Verleihagentur</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>Schweden</t>
+        </is>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>www.youtube.com/watch?v=xDdEWkA15Rg</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>17.10.2020</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Making Montgomery Clift </t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Robert Anderson Clift, Hillary Demmon</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr"/>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>https://www.kino-zeit.de/node/47343</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>https://www.kino-zeit.de/sites/default/files/styles/2560_x_1440_header_/public/2019-08/Making-Montgomery_Clift_filmbild1.jpg</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t xml:space="preserve">missingFILMs </t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>www.youtube.com/watch?v=eJtdIcOR2bM</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>15.10.2020</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Martin Margiela - Mythos der Mode </t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Reiner Holzemer</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr"/>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>https://www.kino-zeit.de/node/48816</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>https://www.kino-zeit.de/sites/default/files/styles/2560_x_1440_header_/public/2020-02/martin_margiela_in_his_own_words_filmstill.jpg</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>Filmwelt Verleihagentur</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>Deutschland, Belgien</t>
+        </is>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>www.youtube.com/watch?v=EvrQX4POKtg</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>15.10.2020</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Moskau Einfach! </t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Micha Lewinsky</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Miriam Stein, Oriana Schrage, Urs Jucker, Michael Maertens, Mike Müller</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>https://www.kino-zeit.de/node/48285</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>https://www.kino-zeit.de/sites/default/files/styles/2560_x_1440_header_/public/2019-12/moskau_einfach_filmbild1.jpg</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Arsenal Filmverleih GmbH </t>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>Schweiz</t>
+        </is>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>www.youtube.com/watch?v=276LLcUGkq8</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>15.10.2020</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mrs. Taylor's Singing Club </t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>Peter Cattaneo</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>Kristin Scott Thomas, Sharon Horgan, Emma Lowndes, Amy James-Kelly</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>https://www.kino-zeit.de/node/48466</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>https://www.kino-zeit.de/sites/default/files/styles/2560_x_1440_header_/public/2020-01/military-wives-filmbild1.jpg</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>Leonine</t>
+        </is>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>Großbritannien</t>
+        </is>
+      </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>www.youtube.com/watch?v=BmDav7mUjMc</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>15.10.2020</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Oeconomia </t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>Carmen Losmann</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr"/>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>https://www.kino-zeit.de/node/48739</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>https://www.kino-zeit.de/sites/default/files/styles/2560_x_1440_header_/public/2020-02/Oeconomia.jpg</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>Neue Visionen Filmverleih GmbH</t>
+        </is>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>Deutschland</t>
+        </is>
+      </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>www.youtube.com/watch?v=RKT_g14MSus</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>15.10.2020</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Rojo - Wenn alle schweigen, ist keiner unschuldig </t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>Benjámin Naishtat</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>Darío Grandinetti, Andrea Frigerio, Alfredo Castro</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>https://www.kino-zeit.de/node/43353</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>https://www.kino-zeit.de/sites/default/files/styles/2560_x_1440_header_/public/2018-08/rojo-filmbild1.jpg</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>Cine Global Filmverleih</t>
+        </is>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>Argentinien, Deutschland</t>
+        </is>
+      </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>www.youtube.com/watch?v=4QhqxLA3aH4</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>15.10.2020</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sag du es mir </t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>Michael Fetter Nathansky</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>Christina Große, Marc Ben Puch, Gisa Flake, Hendrik Arnst, Patrick Heinrich, Walid Al-Atiyat</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>https://www.kino-zeit.de/node/48412</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>https://www.kino-zeit.de/sites/default/files/styles/2560_x_1440_header_/public/2020-08/sagduesmir_filmstill_04.jpg</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t xml:space="preserve">missingFILMs </t>
+        </is>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>Deutschland</t>
+        </is>
+      </c>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t>www.youtube.com/watch?v=UerHnKI8xZs</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>15.10.2020</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Tod auf dem Nil </t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>Kenneth Branagh</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>Kenneth Branagh, Gal Gadot, Armie Hammer, Annette Bening, Sophie Okonedo, Russell Brand, Dawn French</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>https://www.kino-zeit.de/node/49615</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>https://www.kino-zeit.de/sites/default/files/styles/2560_x_1440_header_/public/2020-08/tod-auf-dem-nil-1.jpg</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The Walt Disney Company (Germany) GmbH </t>
+        </is>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t>www.youtube.com/watch?v=npTTR2LDFGI</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>15.10.2020</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Von Liebe und Krieg </t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>Kasper Torsting</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>Tom Wlaschiha, Ulrich Thomsen, Thure Lindhardt, Natalie Madueño, Sebastian Jessen</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>https://www.kino-zeit.de/node/50268</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>https://www.kino-zeit.de/sites/default/files/styles/2560_x_1440_header_/public/2020-09/l-u-k.jpg</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>Tamtam Film</t>
+        </is>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>Dänemark, Deutschland, Tschechische Republik</t>
+        </is>
+      </c>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t>www.youtube.com/watch?v=t406bUnfYGo</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>22.10.2020</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Bohnenstange </t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>Kantemir Balagov</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr"/>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>https://www.kino-zeit.de/node/46389</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>https://www.kino-zeit.de/sites/default/files/styles/2560_x_1440_header_/public/2019-05/beanpole-filmbild1.jpg</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>eksystent distribution filmverleih</t>
+        </is>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>Russland</t>
+        </is>
+      </c>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>www.youtube.com/watch?v=PpUx8cxC4RQ</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>22.10.2020</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cortex </t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>Moritz Bleibtreu</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>Moritz Bleibtreu, Jannis Niewöhner, Wotan Wilke Möhring, Nadja Uhl, Nicholas Ofczarek</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>https://www.kino-zeit.de/node/50644</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>https://www.kino-zeit.de/sites/default/files/styles/2560_x_1440_header_/public/2020-08/rev-1-ger_cortex_szenenbilder_dscf1872_high_res_jpeg.jpeg</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>Warner Bros.</t>
+        </is>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>Deutschland</t>
+        </is>
+      </c>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>www.youtube.com/watch?v=1rPsZmICIn4</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>22.10.2020</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Die Stimme des Regenwaldes </t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>Niklaus Hilber</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>Sven Schelker, Charlotte Heinimann, Matthew Crowley, Daniel Ludwig</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>https://www.kino-zeit.de/node/47764</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>https://www.kino-zeit.de/sites/default/files/styles/2560_x_1440_header_/public/2019-10/bruno-manser-filmbild1.jpg</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>Camino Filmverleih GmbH</t>
+        </is>
+      </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>Schweiz, Österreich</t>
+        </is>
+      </c>
+      <c r="J42" t="inlineStr">
+        <is>
+          <t>www.youtube.com/watch?v=8B8O2qNezmE</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>22.10.2020</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ema </t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>Pablo Larrain</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>Gael Garcia Bernal, Mariana Di Girolamo, Santiago Cabrera, Mariana Loyola</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>https://www.kino-zeit.de/node/44753</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>https://www.kino-zeit.de/sites/default/files/styles/2560_x_1440_header_/public/2020-08/ema_filmstill_09.jpg</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>Koch Films GmbH, Studiocanal</t>
+        </is>
+      </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>Chile</t>
+        </is>
+      </c>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t>www.youtube.com/watch?v=Ft79LOIXlfo</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>22.10.2020</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Kajillionaire </t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>Miranda July</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>Evan Rachel Wood, Gina Rodriguez, Richard Jenkins, Debra Winger</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>https://www.kino-zeit.de/node/48596</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>https://www.kino-zeit.de/sites/default/files/styles/2560_x_1440_header_/public/2020-01/Kajillionaire-filmstill.jpg</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>Universal Pictures International Germany GmbH</t>
+        </is>
+      </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+      <c r="J44" t="inlineStr">
+        <is>
+          <t>www.youtube.com/watch?v=xiMPCevu8Wk</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>22.10.2020</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Komm und sieh </t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>Elem Klimow</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr"/>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>https://www.kino-zeit.de/node/50356</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>https://www.kino-zeit.de/sites/default/files/styles/2560_x_1440_header_/public/2020-07/Komm-und-sieh-bild1.jpg</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>Drop-Out Cinema eG</t>
+        </is>
+      </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>UdSSR</t>
+        </is>
+      </c>
+      <c r="J45" t="inlineStr">
+        <is>
+          <t>www.youtube.com/watch?v=8Ab60vCIhh0</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>22.10.2020</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mein Liebhaber, der Esel &amp; ich </t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>Caroline Vignal</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>Laure Calamy, Benjamin Lavernhe, Olivia Côte, Marc Fraize</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>https://www.kino-zeit.de/node/50818</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>https://www.kino-zeit.de/sites/default/files/styles/2560_x_1440_header_/public/2020-09/meinliebhaberdereselundich-1.jpg</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>Capelight Pictures / Wild Bunch</t>
+        </is>
+      </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>Frankreich</t>
+        </is>
+      </c>
+      <c r="J46" t="inlineStr">
+        <is>
+          <t>www.youtube.com/watch?v=s5hgoO27log</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>22.10.2020</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Regeln am Band, bei hoher Geschwindigkeit </t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>Yulia Lokshina</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr"/>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>https://www.kino-zeit.de/node/48463</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>https://www.kino-zeit.de/sites/default/files/styles/2560_x_1440_header_/public/2020-01/REGELNAMBAND_Still_3_%C2%AEwirFILM.png</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>jip Film &amp; Verleih</t>
+        </is>
+      </c>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>Deutschland</t>
+        </is>
+      </c>
+      <c r="J47" t="inlineStr">
+        <is>
+          <t>www.youtube.com/watch?v=nMr_Fwe2yus</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>22.10.2020</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The Beach House </t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>Jeffrey A. Brown</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>Liana Liberato, Noah Le Gros, Jake Weber, Maryann Nagel</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>https://www.kino-zeit.de/node/50175</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>https://www.kino-zeit.de/sites/default/files/styles/2560_x_1440_header_/public/2020-10/thebeachhouse_filmstill_02.jpg</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>Koch Films GmbH, 24 Bilder</t>
+        </is>
+      </c>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+      <c r="J48" t="inlineStr">
+        <is>
+          <t>www.youtube.com/watch?v=1SefWBdRjDU</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>24.10.2020</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The Great Green Wall </t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>Jared P. Scott</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr"/>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>https://www.kino-zeit.de/node/48568</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>https://www.kino-zeit.de/sites/default/files/styles/2560_x_1440_header_/public/2020-01/the-great-green-wall-filmstill5.jpg</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>Weltkino Filmverleih GmbH</t>
+        </is>
+      </c>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>Großbritannien</t>
+        </is>
+      </c>
+      <c r="J49" t="inlineStr">
+        <is>
+          <t>www.youtube.com/watch?v=66EUzT2bG4c</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>22.10.2020</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The Mortuary - Jeder Tod hat eine Geschichte </t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>Ryan Spindell</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>Clancy Brown, Caitlin Fisher, Christine Kilmer, Ema Horvath</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>https://www.kino-zeit.de/node/50782</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>https://www.kino-zeit.de/sites/default/files/styles/2560_x_1440_header_/public/2020-10/mortuary_01.jpg</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>Capelight Pictures, Central Filmverleih</t>
+        </is>
+      </c>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+      <c r="J50" t="inlineStr">
+        <is>
+          <t>www.youtube.com/watch?v=-XZ6Mmbo9SA</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>22.10.2020</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Winterreise </t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>Anders Østergaard, Erzsébet Rácz</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>Bruno Ganz</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>https://www.kino-zeit.de/node/49515</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>https://www.kino-zeit.de/sites/default/files/styles/2560_x_1440_header_/public/2020-04/winterreise1.jpg</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>Real Fiction Filmverleih</t>
+        </is>
+      </c>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>Dänemark, Deutschland</t>
+        </is>
+      </c>
+      <c r="J51" t="inlineStr">
+        <is>
+          <t>www.youtube.com/watch?v=TTU6-nQp5oI</t>
         </is>
       </c>
     </row>

</xml_diff>